<commit_message>
Updated BOM for R1
Updated diode part list to match quantity
</commit_message>
<xml_diff>
--- a/BOM/BOM_RFCX_POWER_BOARD_R1.xlsx
+++ b/BOM/BOM_RFCX_POWER_BOARD_R1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="218">
   <si>
     <t>Qty</t>
   </si>
@@ -249,9 +249,6 @@
     <t>SOD-123</t>
   </si>
   <si>
-    <t>D1, D2</t>
-  </si>
-  <si>
     <t>Diode</t>
   </si>
   <si>
@@ -667,6 +664,15 @@
   </si>
   <si>
     <t>Ex. Price</t>
+  </si>
+  <si>
+    <t>D1, D2, D3</t>
+  </si>
+  <si>
+    <t>SMT JST 2-PIN XHT CONNECTOR</t>
+  </si>
+  <si>
+    <t>691103110002</t>
   </si>
 </sst>
 </file>
@@ -747,7 +753,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -758,23 +764,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -796,6 +793,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1107,7 +1119,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,51 +1129,51 @@
     <col min="3" max="3" width="31.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="8.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="11" customWidth="1"/>
     <col min="7" max="7" width="13.140625" style="2" customWidth="1"/>
     <col min="8" max="8" width="40" style="2" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="24.5703125" style="16" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" style="2" customWidth="1"/>
     <col min="11" max="11" width="24.140625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="36.7109375" style="16" customWidth="1"/>
+    <col min="12" max="12" width="36.7109375" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>201</v>
+      <c r="F1" s="9" t="s">
+        <v>200</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="K1" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>193</v>
+      <c r="J1" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1175,29 +1187,29 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="10">
         <v>0.57099999999999995</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="10">
         <f t="shared" ref="G2:G7" si="0">E2*F2</f>
         <v>0.57099999999999995</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="I2" s="2">
-        <v>691103110002</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="K2" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="J2" s="12" t="s">
         <v>208</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1216,27 +1228,27 @@
       <c r="E3" s="1">
         <v>1</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="10">
         <v>0.57999999999999996</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="10">
         <f t="shared" si="0"/>
         <v>0.57999999999999996</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="J3" s="2" t="s">
+      <c r="I3" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="J3" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="L3" s="16" t="s">
-        <v>170</v>
+      <c r="K3" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1255,27 +1267,27 @@
       <c r="E4" s="1">
         <v>7</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="10">
         <v>8.0600000000000005E-2</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="10">
         <f t="shared" si="0"/>
         <v>0.56420000000000003</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="K4" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="I4" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="L4" s="16" t="s">
-        <v>168</v>
+      <c r="J4" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1294,27 +1306,27 @@
       <c r="E5" s="1">
         <v>1</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="10">
         <v>1.67E-2</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="10">
         <f t="shared" si="0"/>
         <v>1.67E-2</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="K5" s="6" t="s">
+      <c r="I5" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="L5" s="16" t="s">
-        <v>171</v>
+      <c r="J5" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1333,32 +1345,32 @@
       <c r="E6" s="1">
         <v>1</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="10">
         <v>3.9399999999999998E-2</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="10">
         <f t="shared" si="0"/>
         <v>3.9399999999999998E-2</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="K6" s="6" t="s">
+      <c r="I6" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="L6" s="16" t="s">
-        <v>172</v>
+      <c r="J6" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>74</v>
@@ -1372,27 +1384,27 @@
       <c r="E7" s="1">
         <v>3</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="10">
         <v>0.2437</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="10">
         <f t="shared" si="0"/>
         <v>0.73109999999999997</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="I7" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="I7" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="K7" s="6" t="s">
+      <c r="J7" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="L7" s="16" t="s">
-        <v>169</v>
+      <c r="K7" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1411,27 +1423,27 @@
       <c r="E8" s="1">
         <v>1</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="10">
         <v>0.3019</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="10">
         <f t="shared" ref="G8:G31" si="1">E8*F8</f>
         <v>0.3019</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="J8" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>195</v>
+      <c r="K8" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1445,29 +1457,32 @@
         <v>2</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E9" s="1">
         <v>2</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="10">
         <v>9.9099999999999994E-2</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="10">
         <f t="shared" si="1"/>
         <v>0.19819999999999999</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="I9" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="K9" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>206</v>
+      <c r="L9" s="13" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1486,27 +1501,27 @@
       <c r="E10" s="1">
         <v>1</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="10">
         <v>0.13700000000000001</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="10">
         <f t="shared" si="1"/>
         <v>0.13700000000000001</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="J10" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="L10" s="16" t="s">
-        <v>176</v>
+      <c r="K10" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1525,27 +1540,27 @@
       <c r="E11" s="1">
         <v>2</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="10">
         <v>9.4799999999999995E-2</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="10">
         <f t="shared" si="1"/>
         <v>0.18959999999999999</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="J11" s="2" t="s">
+      <c r="I11" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="K11" s="6" t="s">
+      <c r="J11" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="L11" s="16" t="s">
-        <v>173</v>
+      <c r="K11" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1559,32 +1574,32 @@
         <v>68</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E12" s="1">
         <v>2</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="10">
         <v>9.98E-2</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="10">
         <f t="shared" si="1"/>
         <v>0.1996</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="L12" s="16" t="s">
-        <v>175</v>
+        <v>87</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1598,110 +1613,110 @@
         <v>68</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E13" s="1">
         <v>2</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="10">
         <v>0.1331</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="10">
         <f t="shared" si="1"/>
         <v>0.26619999999999999</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="K13" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I13" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="L13" s="16" t="s">
-        <v>174</v>
+      <c r="J13" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E14" s="1">
         <v>2</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="10">
         <v>1.5347999999999999</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="10">
         <f t="shared" si="1"/>
         <v>3.0695999999999999</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="K14" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I14" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="L14" s="16" t="s">
-        <v>178</v>
+      <c r="J14" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="10">
         <v>6.7799999999999999E-2</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="10">
         <f t="shared" si="1"/>
         <v>6.7799999999999999E-2</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="K15" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="L15" s="16" t="s">
-        <v>196</v>
+        <v>83</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1720,27 +1735,27 @@
       <c r="E16" s="1">
         <v>2</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="10">
         <v>0.62160000000000004</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="10">
         <f t="shared" si="1"/>
         <v>1.2432000000000001</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="J16" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="J16" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="L16" s="16" t="s">
-        <v>177</v>
+      <c r="K16" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1759,27 +1774,27 @@
       <c r="E17" s="1">
         <v>4</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="10">
         <v>1.29E-2</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G17" s="10">
         <f t="shared" si="1"/>
         <v>5.16E-2</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="J17" s="7" t="s">
+      <c r="I17" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="K17" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="K17" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="L17" s="16" t="s">
-        <v>192</v>
+      <c r="L17" s="13" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1798,27 +1813,27 @@
       <c r="E18" s="1">
         <v>2</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="10">
         <v>8.8000000000000005E-3</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="10">
         <f t="shared" si="1"/>
         <v>1.7600000000000001E-2</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="K18" s="8" t="s">
+      <c r="I18" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="L18" s="16" t="s">
-        <v>179</v>
+      <c r="J18" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1837,27 +1852,27 @@
       <c r="E19" s="1">
         <v>2</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="10">
         <v>0.60029999999999994</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="10">
         <f t="shared" si="1"/>
         <v>1.2005999999999999</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I19" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="J19" s="2" t="s">
+      <c r="I19" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="K19" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L19" s="16" t="s">
-        <v>180</v>
+      <c r="J19" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1876,27 +1891,27 @@
       <c r="E20" s="1">
         <v>2</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="10">
         <v>0.4304</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="10">
         <f t="shared" si="1"/>
         <v>0.86080000000000001</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I20" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="L20" s="16" t="s">
-        <v>181</v>
+      <c r="I20" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1915,27 +1930,27 @@
       <c r="E21" s="1">
         <v>10</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="10">
         <v>8.6999999999999994E-3</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="10">
         <f t="shared" si="1"/>
         <v>8.6999999999999994E-2</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="K21" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="I21" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="L21" s="16" t="s">
-        <v>182</v>
+      <c r="J21" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="L21" s="13" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1954,27 +1969,27 @@
       <c r="E22" s="1">
         <v>2</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="10">
         <v>7.9899999999999999E-2</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="10">
         <f t="shared" si="1"/>
         <v>0.1598</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="J22" s="2" t="s">
+      <c r="I22" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="K22" s="6" t="s">
+      <c r="J22" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="L22" s="16" t="s">
-        <v>185</v>
+      <c r="K22" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="L22" s="13" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1993,27 +2008,27 @@
       <c r="E23" s="1">
         <v>1</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F23" s="10">
         <v>1.67E-2</v>
       </c>
-      <c r="G23" s="13">
+      <c r="G23" s="10">
         <f t="shared" si="1"/>
         <v>1.67E-2</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="K23" s="8" t="s">
+      <c r="I23" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="L23" s="16" t="s">
-        <v>186</v>
+      <c r="J23" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="L23" s="13" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -2032,27 +2047,27 @@
       <c r="E24" s="1">
         <v>1</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24" s="10">
         <v>1.67E-2</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G24" s="10">
         <f t="shared" si="1"/>
         <v>1.67E-2</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="K24" s="8" t="s">
+      <c r="I24" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="L24" s="16" t="s">
-        <v>186</v>
+      <c r="J24" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="L24" s="13" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2071,27 +2086,27 @@
       <c r="E25" s="1">
         <v>2</v>
       </c>
-      <c r="F25" s="13">
+      <c r="F25" s="10">
         <v>1.29E-2</v>
       </c>
-      <c r="G25" s="13">
+      <c r="G25" s="10">
         <f t="shared" si="1"/>
         <v>2.58E-2</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="J25" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="K25" s="6" t="s">
+      <c r="I25" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="J25" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="L25" s="13" t="s">
         <v>183</v>
-      </c>
-      <c r="L25" s="16" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2110,27 +2125,27 @@
       <c r="E26" s="1">
         <v>1</v>
       </c>
-      <c r="F26" s="13">
+      <c r="F26" s="10">
         <v>8.8000000000000005E-3</v>
       </c>
-      <c r="G26" s="13">
+      <c r="G26" s="10">
         <f t="shared" si="1"/>
         <v>8.8000000000000005E-3</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I26" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="K26" s="8" t="s">
+      <c r="I26" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="L26" s="16" t="s">
-        <v>187</v>
+      <c r="J26" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2149,27 +2164,27 @@
       <c r="E27" s="1">
         <v>1</v>
       </c>
-      <c r="F27" s="13">
+      <c r="F27" s="10">
         <v>8.8000000000000005E-3</v>
       </c>
-      <c r="G27" s="13">
+      <c r="G27" s="10">
         <f t="shared" si="1"/>
         <v>8.8000000000000005E-3</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="K27" s="8" t="s">
+      <c r="I27" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="L27" s="16" t="s">
-        <v>188</v>
+      <c r="J27" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="L27" s="13" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -2188,27 +2203,27 @@
       <c r="E28" s="1">
         <v>2</v>
       </c>
-      <c r="F28" s="13">
+      <c r="F28" s="10">
         <v>4.4400000000000002E-2</v>
       </c>
-      <c r="G28" s="13">
+      <c r="G28" s="10">
         <f t="shared" si="1"/>
         <v>8.8800000000000004E-2</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="K28" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="I28" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="L28" s="16" t="s">
-        <v>189</v>
+      <c r="J28" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="L28" s="13" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -2222,110 +2237,110 @@
         <v>17</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E29" s="1">
         <v>1</v>
       </c>
-      <c r="F29" s="13">
+      <c r="F29" s="10">
         <v>4.4400000000000002E-2</v>
       </c>
-      <c r="G29" s="13">
+      <c r="G29" s="10">
         <f t="shared" si="1"/>
         <v>4.4400000000000002E-2</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="K29" s="8" t="s">
+      <c r="I29" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="L29" s="16" t="s">
-        <v>190</v>
+      <c r="J29" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="L29" s="13" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="D30" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E30" s="1">
         <v>1</v>
       </c>
-      <c r="F30" s="13">
+      <c r="F30" s="10">
         <v>1.7770999999999999</v>
       </c>
-      <c r="G30" s="13">
+      <c r="G30" s="10">
         <f t="shared" si="1"/>
         <v>1.7770999999999999</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K30" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="I30" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="J30" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="L30" s="16" t="s">
-        <v>191</v>
+      <c r="K30" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="L30" s="13" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="D31" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E31" s="2">
         <v>1</v>
       </c>
-      <c r="F31" s="14">
+      <c r="F31" s="11">
         <v>0.46920000000000001</v>
       </c>
-      <c r="G31" s="13">
+      <c r="G31" s="10">
         <f t="shared" si="1"/>
         <v>0.46920000000000001</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I31" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I31" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="J31" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="K31" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="L31" s="12" t="s">
         <v>213</v>
-      </c>
-      <c r="K31" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="L31" s="15" t="s">
-        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -2363,6 +2378,9 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId31"/>
+  <ignoredErrors>
+    <ignoredError sqref="I2" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>